<commit_message>
added test renewal and fixed montecarlo output
</commit_message>
<xml_diff>
--- a/COVID Contagio Argentina v2.0/Input/Input_Simulador.xlsx
+++ b/COVID Contagio Argentina v2.0/Input/Input_Simulador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.brottier\Documents\COVID 19\COVID-19-Simulation-Argentina\COVID Contagio Argentina v2.0\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9D3419-7902-4C3E-A506-648CB5C10ABC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BD1515-0A8D-4134-B90F-D5AF1F18C2E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="3" activeTab="4" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{55AC4C4C-7526-4060-9BB2-10E89010456B}"/>
   </bookViews>
   <sheets>
     <sheet name="Información" sheetId="28" r:id="rId1"/>
@@ -2362,32 +2362,11 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2398,10 +2377,16 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2413,7 +2398,22 @@
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2937,22 +2937,22 @@
   <sheetData>
     <row r="1" spans="2:45" s="9" customFormat="1"/>
     <row r="2" spans="2:45" s="9" customFormat="1" ht="33.75" customHeight="1" thickBot="1">
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="116" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="123"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="123"/>
-      <c r="O2" s="123"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="116"/>
       <c r="Q2" s="57"/>
       <c r="R2" s="57"/>
       <c r="S2" s="57"/>
@@ -2970,248 +2970,248 @@
     </row>
     <row r="3" spans="2:45" ht="15.75" thickTop="1"/>
     <row r="4" spans="2:45" ht="15" customHeight="1">
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="114" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="119"/>
-      <c r="K4" s="119"/>
-      <c r="L4" s="119"/>
-      <c r="M4" s="119"/>
-      <c r="N4" s="119"/>
-      <c r="O4" s="119"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
     </row>
     <row r="5" spans="2:45" ht="22.5" customHeight="1">
-      <c r="B5" s="119"/>
-      <c r="C5" s="119"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="119"/>
-      <c r="L5" s="119"/>
-      <c r="M5" s="119"/>
-      <c r="N5" s="119"/>
-      <c r="O5" s="119"/>
-      <c r="Q5" s="127" t="s">
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
+      <c r="I5" s="114"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="114"/>
+      <c r="L5" s="114"/>
+      <c r="M5" s="114"/>
+      <c r="N5" s="114"/>
+      <c r="O5" s="114"/>
+      <c r="Q5" s="121" t="s">
         <v>173</v>
       </c>
-      <c r="R5" s="127"/>
-      <c r="S5" s="127"/>
-      <c r="T5" s="127"/>
-      <c r="U5" s="127"/>
-      <c r="V5" s="127"/>
-      <c r="W5" s="127"/>
-      <c r="X5" s="127"/>
-      <c r="Y5" s="127"/>
-      <c r="Z5" s="127"/>
-      <c r="AA5" s="127"/>
-      <c r="AB5" s="127"/>
-      <c r="AC5" s="127"/>
-      <c r="AD5" s="127"/>
+      <c r="R5" s="121"/>
+      <c r="S5" s="121"/>
+      <c r="T5" s="121"/>
+      <c r="U5" s="121"/>
+      <c r="V5" s="121"/>
+      <c r="W5" s="121"/>
+      <c r="X5" s="121"/>
+      <c r="Y5" s="121"/>
+      <c r="Z5" s="121"/>
+      <c r="AA5" s="121"/>
+      <c r="AB5" s="121"/>
+      <c r="AC5" s="121"/>
+      <c r="AD5" s="121"/>
       <c r="AQ5" s="9"/>
       <c r="AR5" s="9"/>
       <c r="AS5" s="9"/>
     </row>
     <row r="6" spans="2:45">
-      <c r="Q6" s="126" t="s">
+      <c r="Q6" s="120" t="s">
         <v>174</v>
       </c>
-      <c r="R6" s="126"/>
-      <c r="S6" s="126"/>
-      <c r="T6" s="126"/>
-      <c r="U6" s="126"/>
-      <c r="V6" s="126"/>
-      <c r="W6" s="126"/>
-      <c r="X6" s="126"/>
-      <c r="Y6" s="126"/>
-      <c r="Z6" s="126"/>
-      <c r="AA6" s="126"/>
-      <c r="AB6" s="126"/>
-      <c r="AC6" s="126"/>
-      <c r="AD6" s="126"/>
+      <c r="R6" s="120"/>
+      <c r="S6" s="120"/>
+      <c r="T6" s="120"/>
+      <c r="U6" s="120"/>
+      <c r="V6" s="120"/>
+      <c r="W6" s="120"/>
+      <c r="X6" s="120"/>
+      <c r="Y6" s="120"/>
+      <c r="Z6" s="120"/>
+      <c r="AA6" s="120"/>
+      <c r="AB6" s="120"/>
+      <c r="AC6" s="120"/>
+      <c r="AD6" s="120"/>
     </row>
     <row r="7" spans="2:45">
-      <c r="Q7" s="126"/>
-      <c r="R7" s="126"/>
-      <c r="S7" s="126"/>
-      <c r="T7" s="126"/>
-      <c r="U7" s="126"/>
-      <c r="V7" s="126"/>
-      <c r="W7" s="126"/>
-      <c r="X7" s="126"/>
-      <c r="Y7" s="126"/>
-      <c r="Z7" s="126"/>
-      <c r="AA7" s="126"/>
-      <c r="AB7" s="126"/>
-      <c r="AC7" s="126"/>
-      <c r="AD7" s="126"/>
+      <c r="Q7" s="120"/>
+      <c r="R7" s="120"/>
+      <c r="S7" s="120"/>
+      <c r="T7" s="120"/>
+      <c r="U7" s="120"/>
+      <c r="V7" s="120"/>
+      <c r="W7" s="120"/>
+      <c r="X7" s="120"/>
+      <c r="Y7" s="120"/>
+      <c r="Z7" s="120"/>
+      <c r="AA7" s="120"/>
+      <c r="AB7" s="120"/>
+      <c r="AC7" s="120"/>
+      <c r="AD7" s="120"/>
     </row>
     <row r="8" spans="2:45" ht="15" customHeight="1">
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="114" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-      <c r="N8" s="119"/>
-      <c r="O8" s="119"/>
-      <c r="Q8" s="126"/>
-      <c r="R8" s="126"/>
-      <c r="S8" s="126"/>
-      <c r="T8" s="126"/>
-      <c r="U8" s="126"/>
-      <c r="V8" s="126"/>
-      <c r="W8" s="126"/>
-      <c r="X8" s="126"/>
-      <c r="Y8" s="126"/>
-      <c r="Z8" s="126"/>
-      <c r="AA8" s="126"/>
-      <c r="AB8" s="126"/>
-      <c r="AC8" s="126"/>
-      <c r="AD8" s="126"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="114"/>
+      <c r="E8" s="114"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="114"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="114"/>
+      <c r="J8" s="114"/>
+      <c r="K8" s="114"/>
+      <c r="L8" s="114"/>
+      <c r="M8" s="114"/>
+      <c r="N8" s="114"/>
+      <c r="O8" s="114"/>
+      <c r="Q8" s="120"/>
+      <c r="R8" s="120"/>
+      <c r="S8" s="120"/>
+      <c r="T8" s="120"/>
+      <c r="U8" s="120"/>
+      <c r="V8" s="120"/>
+      <c r="W8" s="120"/>
+      <c r="X8" s="120"/>
+      <c r="Y8" s="120"/>
+      <c r="Z8" s="120"/>
+      <c r="AA8" s="120"/>
+      <c r="AB8" s="120"/>
+      <c r="AC8" s="120"/>
+      <c r="AD8" s="120"/>
     </row>
     <row r="9" spans="2:45" ht="17.25" customHeight="1">
-      <c r="B9" s="119"/>
-      <c r="C9" s="119"/>
-      <c r="D9" s="119"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-      <c r="M9" s="119"/>
-      <c r="N9" s="119"/>
-      <c r="O9" s="119"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="114"/>
+      <c r="O9" s="114"/>
     </row>
     <row r="12" spans="2:45" ht="17.25" customHeight="1">
       <c r="D12" s="15" t="s">
         <v>96</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="124" t="s">
+      <c r="I12" s="117" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="125"/>
-      <c r="K12" s="125"/>
-      <c r="L12" s="125"/>
-      <c r="M12" s="125"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="118"/>
+      <c r="L12" s="118"/>
+      <c r="M12" s="118"/>
     </row>
     <row r="13" spans="2:45" ht="17.25">
       <c r="D13" s="11" t="s">
         <v>104</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="125"/>
-      <c r="K13" s="125"/>
-      <c r="L13" s="125"/>
-      <c r="M13" s="125"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="118"/>
+      <c r="K13" s="118"/>
+      <c r="L13" s="118"/>
+      <c r="M13" s="118"/>
     </row>
     <row r="14" spans="2:45" ht="17.25">
       <c r="D14" s="13" t="s">
         <v>97</v>
       </c>
       <c r="H14" s="17"/>
-      <c r="I14" s="124"/>
-      <c r="J14" s="125"/>
-      <c r="K14" s="125"/>
-      <c r="L14" s="125"/>
-      <c r="M14" s="125"/>
+      <c r="I14" s="117"/>
+      <c r="J14" s="118"/>
+      <c r="K14" s="118"/>
+      <c r="L14" s="118"/>
+      <c r="M14" s="118"/>
     </row>
     <row r="15" spans="2:45" ht="17.25" customHeight="1">
       <c r="D15" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="I15" s="124"/>
-      <c r="J15" s="125"/>
-      <c r="K15" s="125"/>
-      <c r="L15" s="125"/>
-      <c r="M15" s="125"/>
+      <c r="I15" s="117"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="118"/>
     </row>
     <row r="17" spans="2:43" ht="17.25" customHeight="1">
       <c r="G17" s="18"/>
-      <c r="I17" s="124" t="s">
+      <c r="I17" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="J17" s="125"/>
-      <c r="K17" s="125"/>
-      <c r="L17" s="125"/>
-      <c r="M17" s="125"/>
+      <c r="J17" s="118"/>
+      <c r="K17" s="118"/>
+      <c r="L17" s="118"/>
+      <c r="M17" s="118"/>
     </row>
     <row r="18" spans="2:43" ht="17.25">
       <c r="D18" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="124"/>
-      <c r="J18" s="125"/>
-      <c r="K18" s="125"/>
-      <c r="L18" s="125"/>
-      <c r="M18" s="125"/>
+      <c r="I18" s="117"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="118"/>
+      <c r="L18" s="118"/>
+      <c r="M18" s="118"/>
     </row>
     <row r="19" spans="2:43" ht="15" customHeight="1">
-      <c r="I19" s="124"/>
-      <c r="J19" s="125"/>
-      <c r="K19" s="125"/>
-      <c r="L19" s="125"/>
-      <c r="M19" s="125"/>
+      <c r="I19" s="117"/>
+      <c r="J19" s="118"/>
+      <c r="K19" s="118"/>
+      <c r="L19" s="118"/>
+      <c r="M19" s="118"/>
     </row>
     <row r="22" spans="2:43">
-      <c r="B22" s="128" t="s">
+      <c r="B22" s="123" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="128"/>
-      <c r="D22" s="128"/>
-      <c r="E22" s="128"/>
-      <c r="F22" s="128"/>
-      <c r="G22" s="128"/>
-      <c r="H22" s="128"/>
-      <c r="I22" s="128"/>
-      <c r="J22" s="128"/>
-      <c r="K22" s="128"/>
-      <c r="L22" s="128"/>
-      <c r="M22" s="128"/>
-      <c r="N22" s="128"/>
-      <c r="O22" s="128"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="123"/>
+      <c r="G22" s="123"/>
+      <c r="H22" s="123"/>
+      <c r="I22" s="123"/>
+      <c r="J22" s="123"/>
+      <c r="K22" s="123"/>
+      <c r="L22" s="123"/>
+      <c r="M22" s="123"/>
+      <c r="N22" s="123"/>
+      <c r="O22" s="123"/>
     </row>
     <row r="23" spans="2:43" ht="15" customHeight="1"/>
     <row r="24" spans="2:43" ht="17.25">
-      <c r="B24" s="114" t="s">
+      <c r="B24" s="122" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="114"/>
-      <c r="H24" s="114"/>
-      <c r="I24" s="114"/>
-      <c r="J24" s="114"/>
-      <c r="K24" s="114"/>
-      <c r="L24" s="114"/>
-      <c r="M24" s="114"/>
-      <c r="N24" s="114"/>
-      <c r="O24" s="114"/>
+      <c r="C24" s="122"/>
+      <c r="D24" s="122"/>
+      <c r="E24" s="122"/>
+      <c r="F24" s="122"/>
+      <c r="G24" s="122"/>
+      <c r="H24" s="122"/>
+      <c r="I24" s="122"/>
+      <c r="J24" s="122"/>
+      <c r="K24" s="122"/>
+      <c r="L24" s="122"/>
+      <c r="M24" s="122"/>
+      <c r="N24" s="122"/>
+      <c r="O24" s="122"/>
     </row>
     <row r="25" spans="2:43">
       <c r="R25" s="23"/>
@@ -3232,37 +3232,37 @@
         <v>96</v>
       </c>
       <c r="R26" s="26"/>
-      <c r="S26" s="131" t="s">
+      <c r="S26" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="T26" s="131"/>
-      <c r="U26" s="131"/>
-      <c r="V26" s="131"/>
-      <c r="W26" s="131"/>
-      <c r="X26" s="131"/>
-      <c r="Y26" s="131"/>
-      <c r="Z26" s="131"/>
-      <c r="AA26" s="131"/>
-      <c r="AB26" s="131"/>
+      <c r="T26" s="127"/>
+      <c r="U26" s="127"/>
+      <c r="V26" s="127"/>
+      <c r="W26" s="127"/>
+      <c r="X26" s="127"/>
+      <c r="Y26" s="127"/>
+      <c r="Z26" s="127"/>
+      <c r="AA26" s="127"/>
+      <c r="AB26" s="127"/>
       <c r="AC26" s="27"/>
     </row>
     <row r="27" spans="2:43" ht="15" customHeight="1">
-      <c r="B27" s="119" t="s">
+      <c r="B27" s="114" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="119"/>
-      <c r="D27" s="119"/>
-      <c r="E27" s="119"/>
-      <c r="F27" s="119"/>
-      <c r="G27" s="119"/>
-      <c r="H27" s="119"/>
-      <c r="I27" s="119"/>
-      <c r="J27" s="119"/>
-      <c r="K27" s="119"/>
-      <c r="L27" s="119"/>
-      <c r="M27" s="119"/>
-      <c r="N27" s="119"/>
-      <c r="O27" s="119"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="114"/>
+      <c r="E27" s="114"/>
+      <c r="F27" s="114"/>
+      <c r="G27" s="114"/>
+      <c r="H27" s="114"/>
+      <c r="I27" s="114"/>
+      <c r="J27" s="114"/>
+      <c r="K27" s="114"/>
+      <c r="L27" s="114"/>
+      <c r="M27" s="114"/>
+      <c r="N27" s="114"/>
+      <c r="O27" s="114"/>
       <c r="R27" s="26"/>
       <c r="S27" s="24"/>
       <c r="T27" s="24"/>
@@ -3287,51 +3287,51 @@
       <c r="AQ27" s="18"/>
     </row>
     <row r="28" spans="2:43" ht="15" customHeight="1">
-      <c r="B28" s="119"/>
-      <c r="C28" s="119"/>
-      <c r="D28" s="119"/>
-      <c r="E28" s="119"/>
-      <c r="F28" s="119"/>
-      <c r="G28" s="119"/>
-      <c r="H28" s="119"/>
-      <c r="I28" s="119"/>
-      <c r="J28" s="119"/>
-      <c r="K28" s="119"/>
-      <c r="L28" s="119"/>
-      <c r="M28" s="119"/>
-      <c r="N28" s="119"/>
-      <c r="O28" s="119"/>
+      <c r="B28" s="114"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="114"/>
+      <c r="E28" s="114"/>
+      <c r="F28" s="114"/>
+      <c r="G28" s="114"/>
+      <c r="H28" s="114"/>
+      <c r="I28" s="114"/>
+      <c r="J28" s="114"/>
+      <c r="K28" s="114"/>
+      <c r="L28" s="114"/>
+      <c r="M28" s="114"/>
+      <c r="N28" s="114"/>
+      <c r="O28" s="114"/>
       <c r="R28" s="26"/>
       <c r="AC28" s="27"/>
     </row>
     <row r="29" spans="2:43" ht="17.25">
-      <c r="B29" s="119"/>
-      <c r="C29" s="119"/>
-      <c r="D29" s="119"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="119"/>
-      <c r="G29" s="119"/>
-      <c r="H29" s="119"/>
-      <c r="I29" s="119"/>
-      <c r="J29" s="119"/>
-      <c r="K29" s="119"/>
-      <c r="L29" s="119"/>
-      <c r="M29" s="119"/>
-      <c r="N29" s="119"/>
-      <c r="O29" s="119"/>
+      <c r="B29" s="114"/>
+      <c r="C29" s="114"/>
+      <c r="D29" s="114"/>
+      <c r="E29" s="114"/>
+      <c r="F29" s="114"/>
+      <c r="G29" s="114"/>
+      <c r="H29" s="114"/>
+      <c r="I29" s="114"/>
+      <c r="J29" s="114"/>
+      <c r="K29" s="114"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="114"/>
+      <c r="N29" s="114"/>
+      <c r="O29" s="114"/>
       <c r="R29" s="26"/>
-      <c r="S29" s="122" t="s">
+      <c r="S29" s="126" t="s">
         <v>107</v>
       </c>
-      <c r="T29" s="122"/>
-      <c r="U29" s="122"/>
-      <c r="V29" s="122"/>
-      <c r="W29" s="122"/>
-      <c r="X29" s="122"/>
-      <c r="Y29" s="122"/>
-      <c r="Z29" s="122"/>
-      <c r="AA29" s="122"/>
-      <c r="AB29" s="122"/>
+      <c r="T29" s="126"/>
+      <c r="U29" s="126"/>
+      <c r="V29" s="126"/>
+      <c r="W29" s="126"/>
+      <c r="X29" s="126"/>
+      <c r="Y29" s="126"/>
+      <c r="Z29" s="126"/>
+      <c r="AA29" s="126"/>
+      <c r="AB29" s="126"/>
       <c r="AC29" s="27"/>
     </row>
     <row r="30" spans="2:43">
@@ -3349,52 +3349,52 @@
       <c r="AC30" s="27"/>
     </row>
     <row r="31" spans="2:43" ht="17.25">
-      <c r="B31" s="119" t="s">
+      <c r="B31" s="114" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="119"/>
-      <c r="D31" s="119"/>
-      <c r="E31" s="119"/>
-      <c r="F31" s="119"/>
-      <c r="G31" s="119"/>
-      <c r="H31" s="119"/>
-      <c r="I31" s="119"/>
-      <c r="J31" s="119"/>
-      <c r="K31" s="119"/>
-      <c r="L31" s="119"/>
-      <c r="M31" s="119"/>
-      <c r="N31" s="119"/>
-      <c r="O31" s="119"/>
+      <c r="C31" s="114"/>
+      <c r="D31" s="114"/>
+      <c r="E31" s="114"/>
+      <c r="F31" s="114"/>
+      <c r="G31" s="114"/>
+      <c r="H31" s="114"/>
+      <c r="I31" s="114"/>
+      <c r="J31" s="114"/>
+      <c r="K31" s="114"/>
+      <c r="L31" s="114"/>
+      <c r="M31" s="114"/>
+      <c r="N31" s="114"/>
+      <c r="O31" s="114"/>
       <c r="R31" s="26"/>
       <c r="S31" s="18"/>
       <c r="T31" s="18"/>
       <c r="U31" s="18"/>
-      <c r="V31" s="129" t="s">
+      <c r="V31" s="124" t="s">
         <v>109</v>
       </c>
-      <c r="W31" s="129"/>
-      <c r="X31" s="129"/>
-      <c r="Y31" s="129"/>
-      <c r="Z31" s="129"/>
+      <c r="W31" s="124"/>
+      <c r="X31" s="124"/>
+      <c r="Y31" s="124"/>
+      <c r="Z31" s="124"/>
       <c r="AA31" s="18"/>
       <c r="AB31" s="18"/>
       <c r="AC31" s="27"/>
     </row>
     <row r="32" spans="2:43" ht="15" customHeight="1">
-      <c r="B32" s="119"/>
-      <c r="C32" s="119"/>
-      <c r="D32" s="119"/>
-      <c r="E32" s="119"/>
-      <c r="F32" s="119"/>
-      <c r="G32" s="119"/>
-      <c r="H32" s="119"/>
-      <c r="I32" s="119"/>
-      <c r="J32" s="119"/>
-      <c r="K32" s="119"/>
-      <c r="L32" s="119"/>
-      <c r="M32" s="119"/>
-      <c r="N32" s="119"/>
-      <c r="O32" s="119"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="114"/>
+      <c r="E32" s="114"/>
+      <c r="F32" s="114"/>
+      <c r="G32" s="114"/>
+      <c r="H32" s="114"/>
+      <c r="I32" s="114"/>
+      <c r="J32" s="114"/>
+      <c r="K32" s="114"/>
+      <c r="L32" s="114"/>
+      <c r="M32" s="114"/>
+      <c r="N32" s="114"/>
+      <c r="O32" s="114"/>
       <c r="R32" s="26"/>
       <c r="S32" s="18"/>
       <c r="T32" s="18"/>
@@ -3409,61 +3409,61 @@
       <c r="AC32" s="27"/>
     </row>
     <row r="33" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B33" s="119" t="s">
+      <c r="B33" s="114" t="s">
         <v>172</v>
       </c>
-      <c r="C33" s="119"/>
-      <c r="D33" s="119"/>
-      <c r="E33" s="119"/>
-      <c r="F33" s="119"/>
-      <c r="G33" s="119"/>
-      <c r="H33" s="119"/>
-      <c r="I33" s="119"/>
-      <c r="J33" s="119"/>
-      <c r="K33" s="119"/>
-      <c r="L33" s="119"/>
-      <c r="M33" s="119"/>
-      <c r="N33" s="119"/>
+      <c r="C33" s="114"/>
+      <c r="D33" s="114"/>
+      <c r="E33" s="114"/>
+      <c r="F33" s="114"/>
+      <c r="G33" s="114"/>
+      <c r="H33" s="114"/>
+      <c r="I33" s="114"/>
+      <c r="J33" s="114"/>
+      <c r="K33" s="114"/>
+      <c r="L33" s="114"/>
+      <c r="M33" s="114"/>
+      <c r="N33" s="114"/>
       <c r="R33" s="26"/>
-      <c r="S33" s="120" t="s">
+      <c r="S33" s="128" t="s">
         <v>108</v>
       </c>
-      <c r="T33" s="120"/>
-      <c r="U33" s="120"/>
-      <c r="V33" s="120"/>
-      <c r="W33" s="120"/>
-      <c r="X33" s="120"/>
-      <c r="Y33" s="120"/>
-      <c r="Z33" s="120"/>
-      <c r="AA33" s="120"/>
-      <c r="AB33" s="120"/>
+      <c r="T33" s="128"/>
+      <c r="U33" s="128"/>
+      <c r="V33" s="128"/>
+      <c r="W33" s="128"/>
+      <c r="X33" s="128"/>
+      <c r="Y33" s="128"/>
+      <c r="Z33" s="128"/>
+      <c r="AA33" s="128"/>
+      <c r="AB33" s="128"/>
       <c r="AC33" s="27"/>
     </row>
     <row r="34" spans="2:32" ht="17.25" customHeight="1">
-      <c r="B34" s="119"/>
-      <c r="C34" s="119"/>
-      <c r="D34" s="119"/>
-      <c r="E34" s="119"/>
-      <c r="F34" s="119"/>
-      <c r="G34" s="119"/>
-      <c r="H34" s="119"/>
-      <c r="I34" s="119"/>
-      <c r="J34" s="119"/>
-      <c r="K34" s="119"/>
-      <c r="L34" s="119"/>
-      <c r="M34" s="119"/>
-      <c r="N34" s="119"/>
+      <c r="B34" s="114"/>
+      <c r="C34" s="114"/>
+      <c r="D34" s="114"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="114"/>
+      <c r="G34" s="114"/>
+      <c r="H34" s="114"/>
+      <c r="I34" s="114"/>
+      <c r="J34" s="114"/>
+      <c r="K34" s="114"/>
+      <c r="L34" s="114"/>
+      <c r="M34" s="114"/>
+      <c r="N34" s="114"/>
       <c r="R34" s="26"/>
-      <c r="S34" s="120"/>
-      <c r="T34" s="120"/>
-      <c r="U34" s="120"/>
-      <c r="V34" s="120"/>
-      <c r="W34" s="120"/>
-      <c r="X34" s="120"/>
-      <c r="Y34" s="120"/>
-      <c r="Z34" s="120"/>
-      <c r="AA34" s="120"/>
-      <c r="AB34" s="120"/>
+      <c r="S34" s="128"/>
+      <c r="T34" s="128"/>
+      <c r="U34" s="128"/>
+      <c r="V34" s="128"/>
+      <c r="W34" s="128"/>
+      <c r="X34" s="128"/>
+      <c r="Y34" s="128"/>
+      <c r="Z34" s="128"/>
+      <c r="AA34" s="128"/>
+      <c r="AB34" s="128"/>
       <c r="AC34" s="27"/>
     </row>
     <row r="35" spans="2:32">
@@ -3501,67 +3501,67 @@
     </row>
     <row r="37" spans="2:32">
       <c r="R37" s="26"/>
-      <c r="S37" s="121" t="s">
+      <c r="S37" s="129" t="s">
         <v>111</v>
       </c>
-      <c r="T37" s="121"/>
-      <c r="U37" s="121"/>
-      <c r="V37" s="121"/>
-      <c r="W37" s="121"/>
-      <c r="X37" s="121"/>
-      <c r="Y37" s="121"/>
-      <c r="Z37" s="121"/>
-      <c r="AA37" s="121"/>
-      <c r="AB37" s="121"/>
+      <c r="T37" s="129"/>
+      <c r="U37" s="129"/>
+      <c r="V37" s="129"/>
+      <c r="W37" s="129"/>
+      <c r="X37" s="129"/>
+      <c r="Y37" s="129"/>
+      <c r="Z37" s="129"/>
+      <c r="AA37" s="129"/>
+      <c r="AB37" s="129"/>
       <c r="AC37" s="27"/>
       <c r="AF37" s="9"/>
     </row>
     <row r="38" spans="2:32">
-      <c r="B38" s="119" t="s">
+      <c r="B38" s="114" t="s">
         <v>142</v>
       </c>
-      <c r="C38" s="119"/>
-      <c r="D38" s="119"/>
-      <c r="E38" s="119"/>
-      <c r="F38" s="119"/>
-      <c r="G38" s="119"/>
-      <c r="H38" s="119"/>
-      <c r="I38" s="119"/>
-      <c r="J38" s="119"/>
-      <c r="K38" s="119"/>
-      <c r="L38" s="119"/>
-      <c r="M38" s="119"/>
-      <c r="N38" s="119"/>
-      <c r="O38" s="119"/>
+      <c r="C38" s="114"/>
+      <c r="D38" s="114"/>
+      <c r="E38" s="114"/>
+      <c r="F38" s="114"/>
+      <c r="G38" s="114"/>
+      <c r="H38" s="114"/>
+      <c r="I38" s="114"/>
+      <c r="J38" s="114"/>
+      <c r="K38" s="114"/>
+      <c r="L38" s="114"/>
+      <c r="M38" s="114"/>
+      <c r="N38" s="114"/>
+      <c r="O38" s="114"/>
       <c r="R38" s="26"/>
-      <c r="S38" s="121"/>
-      <c r="T38" s="121"/>
-      <c r="U38" s="121"/>
-      <c r="V38" s="121"/>
-      <c r="W38" s="121"/>
-      <c r="X38" s="121"/>
-      <c r="Y38" s="121"/>
-      <c r="Z38" s="121"/>
-      <c r="AA38" s="121"/>
-      <c r="AB38" s="121"/>
+      <c r="S38" s="129"/>
+      <c r="T38" s="129"/>
+      <c r="U38" s="129"/>
+      <c r="V38" s="129"/>
+      <c r="W38" s="129"/>
+      <c r="X38" s="129"/>
+      <c r="Y38" s="129"/>
+      <c r="Z38" s="129"/>
+      <c r="AA38" s="129"/>
+      <c r="AB38" s="129"/>
       <c r="AC38" s="27"/>
       <c r="AF38" s="9"/>
     </row>
     <row r="39" spans="2:32">
-      <c r="B39" s="119"/>
-      <c r="C39" s="119"/>
-      <c r="D39" s="119"/>
-      <c r="E39" s="119"/>
-      <c r="F39" s="119"/>
-      <c r="G39" s="119"/>
-      <c r="H39" s="119"/>
-      <c r="I39" s="119"/>
-      <c r="J39" s="119"/>
-      <c r="K39" s="119"/>
-      <c r="L39" s="119"/>
-      <c r="M39" s="119"/>
-      <c r="N39" s="119"/>
-      <c r="O39" s="119"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="114"/>
+      <c r="D39" s="114"/>
+      <c r="E39" s="114"/>
+      <c r="F39" s="114"/>
+      <c r="G39" s="114"/>
+      <c r="H39" s="114"/>
+      <c r="I39" s="114"/>
+      <c r="J39" s="114"/>
+      <c r="K39" s="114"/>
+      <c r="L39" s="114"/>
+      <c r="M39" s="114"/>
+      <c r="N39" s="114"/>
+      <c r="O39" s="114"/>
       <c r="R39" s="26"/>
       <c r="S39" s="18"/>
       <c r="T39" s="19"/>
@@ -3581,34 +3581,34 @@
       <c r="S40" s="18"/>
       <c r="T40" s="19"/>
       <c r="U40" s="19"/>
-      <c r="V40" s="130" t="s">
+      <c r="V40" s="125" t="s">
         <v>110</v>
       </c>
-      <c r="W40" s="130"/>
-      <c r="X40" s="130"/>
-      <c r="Y40" s="130"/>
-      <c r="Z40" s="130"/>
+      <c r="W40" s="125"/>
+      <c r="X40" s="125"/>
+      <c r="Y40" s="125"/>
+      <c r="Z40" s="125"/>
       <c r="AA40" s="19"/>
       <c r="AB40" s="19"/>
       <c r="AC40" s="27"/>
     </row>
     <row r="41" spans="2:32" ht="17.25">
-      <c r="B41" s="114" t="s">
+      <c r="B41" s="122" t="s">
         <v>104</v>
       </c>
-      <c r="C41" s="114"/>
-      <c r="D41" s="114"/>
-      <c r="E41" s="114"/>
-      <c r="F41" s="114"/>
-      <c r="G41" s="114"/>
-      <c r="H41" s="114"/>
-      <c r="I41" s="114"/>
-      <c r="J41" s="114"/>
-      <c r="K41" s="114"/>
-      <c r="L41" s="114"/>
-      <c r="M41" s="114"/>
-      <c r="N41" s="114"/>
-      <c r="O41" s="114"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="122"/>
+      <c r="E41" s="122"/>
+      <c r="F41" s="122"/>
+      <c r="G41" s="122"/>
+      <c r="H41" s="122"/>
+      <c r="I41" s="122"/>
+      <c r="J41" s="122"/>
+      <c r="K41" s="122"/>
+      <c r="L41" s="122"/>
+      <c r="M41" s="122"/>
+      <c r="N41" s="122"/>
+      <c r="O41" s="122"/>
       <c r="R41" s="26"/>
       <c r="S41" s="18"/>
       <c r="T41" s="18"/>
@@ -3624,18 +3624,18 @@
     </row>
     <row r="42" spans="2:32" ht="17.25">
       <c r="R42" s="26"/>
-      <c r="S42" s="122" t="s">
+      <c r="S42" s="126" t="s">
         <v>112</v>
       </c>
-      <c r="T42" s="122"/>
-      <c r="U42" s="122"/>
-      <c r="V42" s="122"/>
-      <c r="W42" s="122"/>
-      <c r="X42" s="122"/>
-      <c r="Y42" s="122"/>
-      <c r="Z42" s="122"/>
-      <c r="AA42" s="122"/>
-      <c r="AB42" s="122"/>
+      <c r="T42" s="126"/>
+      <c r="U42" s="126"/>
+      <c r="V42" s="126"/>
+      <c r="W42" s="126"/>
+      <c r="X42" s="126"/>
+      <c r="Y42" s="126"/>
+      <c r="Z42" s="126"/>
+      <c r="AA42" s="126"/>
+      <c r="AB42" s="126"/>
       <c r="AC42" s="27"/>
     </row>
     <row r="43" spans="2:32" ht="17.25">
@@ -3670,63 +3670,63 @@
       <c r="AC44" s="27"/>
     </row>
     <row r="45" spans="2:32">
-      <c r="B45" s="119" t="s">
+      <c r="B45" s="114" t="s">
         <v>143</v>
       </c>
-      <c r="C45" s="119"/>
-      <c r="D45" s="119"/>
-      <c r="E45" s="119"/>
-      <c r="F45" s="119"/>
-      <c r="G45" s="119"/>
-      <c r="H45" s="119"/>
-      <c r="I45" s="119"/>
-      <c r="J45" s="119"/>
-      <c r="K45" s="119"/>
-      <c r="L45" s="119"/>
-      <c r="M45" s="119"/>
-      <c r="N45" s="119"/>
-      <c r="O45" s="119"/>
+      <c r="C45" s="114"/>
+      <c r="D45" s="114"/>
+      <c r="E45" s="114"/>
+      <c r="F45" s="114"/>
+      <c r="G45" s="114"/>
+      <c r="H45" s="114"/>
+      <c r="I45" s="114"/>
+      <c r="J45" s="114"/>
+      <c r="K45" s="114"/>
+      <c r="L45" s="114"/>
+      <c r="M45" s="114"/>
+      <c r="N45" s="114"/>
+      <c r="O45" s="114"/>
       <c r="R45" s="26"/>
-      <c r="S45" s="120" t="s">
+      <c r="S45" s="128" t="s">
         <v>113</v>
       </c>
-      <c r="T45" s="120"/>
-      <c r="U45" s="120"/>
-      <c r="V45" s="120"/>
-      <c r="W45" s="120"/>
-      <c r="X45" s="120"/>
-      <c r="Y45" s="120"/>
-      <c r="Z45" s="120"/>
-      <c r="AA45" s="120"/>
-      <c r="AB45" s="120"/>
+      <c r="T45" s="128"/>
+      <c r="U45" s="128"/>
+      <c r="V45" s="128"/>
+      <c r="W45" s="128"/>
+      <c r="X45" s="128"/>
+      <c r="Y45" s="128"/>
+      <c r="Z45" s="128"/>
+      <c r="AA45" s="128"/>
+      <c r="AB45" s="128"/>
       <c r="AC45" s="27"/>
     </row>
     <row r="46" spans="2:32" ht="15" customHeight="1">
-      <c r="B46" s="119"/>
-      <c r="C46" s="119"/>
-      <c r="D46" s="119"/>
-      <c r="E46" s="119"/>
-      <c r="F46" s="119"/>
-      <c r="G46" s="119"/>
-      <c r="H46" s="119"/>
-      <c r="I46" s="119"/>
-      <c r="J46" s="119"/>
-      <c r="K46" s="119"/>
-      <c r="L46" s="119"/>
-      <c r="M46" s="119"/>
-      <c r="N46" s="119"/>
-      <c r="O46" s="119"/>
+      <c r="B46" s="114"/>
+      <c r="C46" s="114"/>
+      <c r="D46" s="114"/>
+      <c r="E46" s="114"/>
+      <c r="F46" s="114"/>
+      <c r="G46" s="114"/>
+      <c r="H46" s="114"/>
+      <c r="I46" s="114"/>
+      <c r="J46" s="114"/>
+      <c r="K46" s="114"/>
+      <c r="L46" s="114"/>
+      <c r="M46" s="114"/>
+      <c r="N46" s="114"/>
+      <c r="O46" s="114"/>
       <c r="R46" s="26"/>
-      <c r="S46" s="120"/>
-      <c r="T46" s="120"/>
-      <c r="U46" s="120"/>
-      <c r="V46" s="120"/>
-      <c r="W46" s="120"/>
-      <c r="X46" s="120"/>
-      <c r="Y46" s="120"/>
-      <c r="Z46" s="120"/>
-      <c r="AA46" s="120"/>
-      <c r="AB46" s="120"/>
+      <c r="S46" s="128"/>
+      <c r="T46" s="128"/>
+      <c r="U46" s="128"/>
+      <c r="V46" s="128"/>
+      <c r="W46" s="128"/>
+      <c r="X46" s="128"/>
+      <c r="Y46" s="128"/>
+      <c r="Z46" s="128"/>
+      <c r="AA46" s="128"/>
+      <c r="AB46" s="128"/>
       <c r="AC46" s="27"/>
     </row>
     <row r="47" spans="2:32" ht="15" customHeight="1">
@@ -3751,13 +3751,13 @@
       <c r="S48" s="18"/>
       <c r="T48" s="18"/>
       <c r="U48" s="18"/>
-      <c r="V48" s="117" t="s">
+      <c r="V48" s="131" t="s">
         <v>114</v>
       </c>
-      <c r="W48" s="117"/>
-      <c r="X48" s="117"/>
-      <c r="Y48" s="117"/>
-      <c r="Z48" s="117"/>
+      <c r="W48" s="131"/>
+      <c r="X48" s="131"/>
+      <c r="Y48" s="131"/>
+      <c r="Z48" s="131"/>
       <c r="AA48" s="18"/>
       <c r="AB48" s="18"/>
       <c r="AC48" s="27"/>
@@ -3777,52 +3777,52 @@
       <c r="AC49" s="27"/>
     </row>
     <row r="50" spans="2:43">
-      <c r="B50" s="119" t="s">
+      <c r="B50" s="114" t="s">
         <v>145</v>
       </c>
-      <c r="C50" s="119"/>
-      <c r="D50" s="119"/>
-      <c r="E50" s="119"/>
-      <c r="F50" s="119"/>
-      <c r="G50" s="119"/>
-      <c r="H50" s="119"/>
-      <c r="I50" s="119"/>
-      <c r="J50" s="119"/>
-      <c r="K50" s="119"/>
-      <c r="L50" s="119"/>
-      <c r="M50" s="119"/>
-      <c r="N50" s="119"/>
-      <c r="O50" s="119"/>
+      <c r="C50" s="114"/>
+      <c r="D50" s="114"/>
+      <c r="E50" s="114"/>
+      <c r="F50" s="114"/>
+      <c r="G50" s="114"/>
+      <c r="H50" s="114"/>
+      <c r="I50" s="114"/>
+      <c r="J50" s="114"/>
+      <c r="K50" s="114"/>
+      <c r="L50" s="114"/>
+      <c r="M50" s="114"/>
+      <c r="N50" s="114"/>
+      <c r="O50" s="114"/>
       <c r="R50" s="26"/>
-      <c r="S50" s="118" t="s">
+      <c r="S50" s="119" t="s">
         <v>115</v>
       </c>
-      <c r="T50" s="118"/>
-      <c r="U50" s="118"/>
-      <c r="V50" s="118"/>
-      <c r="W50" s="118"/>
-      <c r="X50" s="118"/>
-      <c r="Y50" s="118"/>
-      <c r="Z50" s="118"/>
-      <c r="AA50" s="118"/>
-      <c r="AB50" s="118"/>
+      <c r="T50" s="119"/>
+      <c r="U50" s="119"/>
+      <c r="V50" s="119"/>
+      <c r="W50" s="119"/>
+      <c r="X50" s="119"/>
+      <c r="Y50" s="119"/>
+      <c r="Z50" s="119"/>
+      <c r="AA50" s="119"/>
+      <c r="AB50" s="119"/>
       <c r="AC50" s="27"/>
     </row>
     <row r="51" spans="2:43" ht="15" customHeight="1">
-      <c r="B51" s="119"/>
-      <c r="C51" s="119"/>
-      <c r="D51" s="119"/>
-      <c r="E51" s="119"/>
-      <c r="F51" s="119"/>
-      <c r="G51" s="119"/>
-      <c r="H51" s="119"/>
-      <c r="I51" s="119"/>
-      <c r="J51" s="119"/>
-      <c r="K51" s="119"/>
-      <c r="L51" s="119"/>
-      <c r="M51" s="119"/>
-      <c r="N51" s="119"/>
-      <c r="O51" s="119"/>
+      <c r="B51" s="114"/>
+      <c r="C51" s="114"/>
+      <c r="D51" s="114"/>
+      <c r="E51" s="114"/>
+      <c r="F51" s="114"/>
+      <c r="G51" s="114"/>
+      <c r="H51" s="114"/>
+      <c r="I51" s="114"/>
+      <c r="J51" s="114"/>
+      <c r="K51" s="114"/>
+      <c r="L51" s="114"/>
+      <c r="M51" s="114"/>
+      <c r="N51" s="114"/>
+      <c r="O51" s="114"/>
       <c r="R51" s="26"/>
       <c r="S51" s="18"/>
       <c r="T51" s="18"/>
@@ -3838,18 +3838,18 @@
     </row>
     <row r="52" spans="2:43">
       <c r="R52" s="26"/>
-      <c r="S52" s="118" t="s">
+      <c r="S52" s="119" t="s">
         <v>116</v>
       </c>
-      <c r="T52" s="118"/>
-      <c r="U52" s="118"/>
-      <c r="V52" s="118"/>
-      <c r="W52" s="118"/>
-      <c r="X52" s="118"/>
-      <c r="Y52" s="118"/>
-      <c r="Z52" s="118"/>
-      <c r="AA52" s="118"/>
-      <c r="AB52" s="118"/>
+      <c r="T52" s="119"/>
+      <c r="U52" s="119"/>
+      <c r="V52" s="119"/>
+      <c r="W52" s="119"/>
+      <c r="X52" s="119"/>
+      <c r="Y52" s="119"/>
+      <c r="Z52" s="119"/>
+      <c r="AA52" s="119"/>
+      <c r="AB52" s="119"/>
       <c r="AC52" s="27"/>
     </row>
     <row r="53" spans="2:43" ht="15.75" customHeight="1">
@@ -3857,16 +3857,16 @@
         <v>147</v>
       </c>
       <c r="R53" s="26"/>
-      <c r="S53" s="118"/>
-      <c r="T53" s="118"/>
-      <c r="U53" s="118"/>
-      <c r="V53" s="118"/>
-      <c r="W53" s="118"/>
-      <c r="X53" s="118"/>
-      <c r="Y53" s="118"/>
-      <c r="Z53" s="118"/>
-      <c r="AA53" s="118"/>
-      <c r="AB53" s="118"/>
+      <c r="S53" s="119"/>
+      <c r="T53" s="119"/>
+      <c r="U53" s="119"/>
+      <c r="V53" s="119"/>
+      <c r="W53" s="119"/>
+      <c r="X53" s="119"/>
+      <c r="Y53" s="119"/>
+      <c r="Z53" s="119"/>
+      <c r="AA53" s="119"/>
+      <c r="AB53" s="119"/>
       <c r="AC53" s="27"/>
       <c r="AH53" s="22"/>
       <c r="AI53" s="22"/>
@@ -3894,22 +3894,22 @@
       <c r="AC54" s="27"/>
     </row>
     <row r="55" spans="2:43">
-      <c r="B55" s="119" t="s">
+      <c r="B55" s="114" t="s">
         <v>154</v>
       </c>
-      <c r="C55" s="119"/>
-      <c r="D55" s="119"/>
-      <c r="E55" s="119"/>
-      <c r="F55" s="119"/>
-      <c r="G55" s="119"/>
-      <c r="H55" s="119"/>
-      <c r="I55" s="119"/>
-      <c r="J55" s="119"/>
-      <c r="K55" s="119"/>
-      <c r="L55" s="119"/>
-      <c r="M55" s="119"/>
-      <c r="N55" s="119"/>
-      <c r="O55" s="119"/>
+      <c r="C55" s="114"/>
+      <c r="D55" s="114"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="114"/>
+      <c r="G55" s="114"/>
+      <c r="H55" s="114"/>
+      <c r="I55" s="114"/>
+      <c r="J55" s="114"/>
+      <c r="K55" s="114"/>
+      <c r="L55" s="114"/>
+      <c r="M55" s="114"/>
+      <c r="N55" s="114"/>
+      <c r="O55" s="114"/>
       <c r="R55" s="28"/>
       <c r="S55" s="29"/>
       <c r="T55" s="29"/>
@@ -3924,272 +3924,272 @@
       <c r="AC55" s="30"/>
     </row>
     <row r="56" spans="2:43">
-      <c r="B56" s="119"/>
-      <c r="C56" s="119"/>
-      <c r="D56" s="119"/>
-      <c r="E56" s="119"/>
-      <c r="F56" s="119"/>
-      <c r="G56" s="119"/>
-      <c r="H56" s="119"/>
-      <c r="I56" s="119"/>
-      <c r="J56" s="119"/>
-      <c r="K56" s="119"/>
-      <c r="L56" s="119"/>
-      <c r="M56" s="119"/>
-      <c r="N56" s="119"/>
-      <c r="O56" s="119"/>
+      <c r="B56" s="114"/>
+      <c r="C56" s="114"/>
+      <c r="D56" s="114"/>
+      <c r="E56" s="114"/>
+      <c r="F56" s="114"/>
+      <c r="G56" s="114"/>
+      <c r="H56" s="114"/>
+      <c r="I56" s="114"/>
+      <c r="J56" s="114"/>
+      <c r="K56" s="114"/>
+      <c r="L56" s="114"/>
+      <c r="M56" s="114"/>
+      <c r="N56" s="114"/>
+      <c r="O56" s="114"/>
     </row>
     <row r="58" spans="2:43" ht="17.25">
-      <c r="B58" s="114" t="s">
+      <c r="B58" s="122" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="114"/>
-      <c r="D58" s="114"/>
-      <c r="E58" s="114"/>
-      <c r="F58" s="114"/>
-      <c r="G58" s="114"/>
-      <c r="H58" s="114"/>
-      <c r="I58" s="114"/>
-      <c r="J58" s="114"/>
-      <c r="K58" s="114"/>
-      <c r="L58" s="114"/>
-      <c r="M58" s="114"/>
-      <c r="N58" s="114"/>
-      <c r="O58" s="114"/>
-      <c r="Q58" s="115" t="s">
+      <c r="C58" s="122"/>
+      <c r="D58" s="122"/>
+      <c r="E58" s="122"/>
+      <c r="F58" s="122"/>
+      <c r="G58" s="122"/>
+      <c r="H58" s="122"/>
+      <c r="I58" s="122"/>
+      <c r="J58" s="122"/>
+      <c r="K58" s="122"/>
+      <c r="L58" s="122"/>
+      <c r="M58" s="122"/>
+      <c r="N58" s="122"/>
+      <c r="O58" s="122"/>
+      <c r="Q58" s="130" t="s">
         <v>169</v>
       </c>
-      <c r="R58" s="115"/>
-      <c r="S58" s="115"/>
-      <c r="T58" s="115"/>
-      <c r="U58" s="115"/>
-      <c r="V58" s="115"/>
-      <c r="W58" s="115"/>
-      <c r="X58" s="115"/>
-      <c r="Y58" s="115"/>
-      <c r="Z58" s="115"/>
-      <c r="AA58" s="115"/>
-      <c r="AB58" s="115"/>
-      <c r="AC58" s="115"/>
-      <c r="AD58" s="115"/>
+      <c r="R58" s="130"/>
+      <c r="S58" s="130"/>
+      <c r="T58" s="130"/>
+      <c r="U58" s="130"/>
+      <c r="V58" s="130"/>
+      <c r="W58" s="130"/>
+      <c r="X58" s="130"/>
+      <c r="Y58" s="130"/>
+      <c r="Z58" s="130"/>
+      <c r="AA58" s="130"/>
+      <c r="AB58" s="130"/>
+      <c r="AC58" s="130"/>
+      <c r="AD58" s="130"/>
     </row>
     <row r="60" spans="2:43" ht="17.25">
-      <c r="B60" s="116" t="s">
+      <c r="B60" s="115" t="s">
         <v>198</v>
       </c>
-      <c r="C60" s="116"/>
-      <c r="D60" s="116"/>
-      <c r="E60" s="116"/>
-      <c r="F60" s="116"/>
-      <c r="G60" s="116"/>
-      <c r="H60" s="116"/>
-      <c r="I60" s="116"/>
-      <c r="J60" s="116"/>
-      <c r="K60" s="116"/>
-      <c r="L60" s="116"/>
-      <c r="M60" s="116"/>
-      <c r="N60" s="116"/>
-      <c r="O60" s="116"/>
+      <c r="C60" s="115"/>
+      <c r="D60" s="115"/>
+      <c r="E60" s="115"/>
+      <c r="F60" s="115"/>
+      <c r="G60" s="115"/>
+      <c r="H60" s="115"/>
+      <c r="I60" s="115"/>
+      <c r="J60" s="115"/>
+      <c r="K60" s="115"/>
+      <c r="L60" s="115"/>
+      <c r="M60" s="115"/>
+      <c r="N60" s="115"/>
+      <c r="O60" s="115"/>
       <c r="Q60" s="20" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="61" spans="2:43">
-      <c r="B61" s="116"/>
-      <c r="C61" s="116"/>
-      <c r="D61" s="116"/>
-      <c r="E61" s="116"/>
-      <c r="F61" s="116"/>
-      <c r="G61" s="116"/>
-      <c r="H61" s="116"/>
-      <c r="I61" s="116"/>
-      <c r="J61" s="116"/>
-      <c r="K61" s="116"/>
-      <c r="L61" s="116"/>
-      <c r="M61" s="116"/>
-      <c r="N61" s="116"/>
-      <c r="O61" s="116"/>
+      <c r="B61" s="115"/>
+      <c r="C61" s="115"/>
+      <c r="D61" s="115"/>
+      <c r="E61" s="115"/>
+      <c r="F61" s="115"/>
+      <c r="G61" s="115"/>
+      <c r="H61" s="115"/>
+      <c r="I61" s="115"/>
+      <c r="J61" s="115"/>
+      <c r="K61" s="115"/>
+      <c r="L61" s="115"/>
+      <c r="M61" s="115"/>
+      <c r="N61" s="115"/>
+      <c r="O61" s="115"/>
     </row>
     <row r="62" spans="2:43">
-      <c r="Q62" s="119" t="s">
+      <c r="Q62" s="114" t="s">
         <v>195</v>
       </c>
-      <c r="R62" s="119"/>
-      <c r="S62" s="119"/>
-      <c r="T62" s="119"/>
-      <c r="U62" s="119"/>
-      <c r="V62" s="119"/>
-      <c r="W62" s="119"/>
-      <c r="X62" s="119"/>
-      <c r="Y62" s="119"/>
-      <c r="Z62" s="119"/>
-      <c r="AA62" s="119"/>
-      <c r="AB62" s="119"/>
-      <c r="AC62" s="119"/>
-      <c r="AD62" s="119"/>
+      <c r="R62" s="114"/>
+      <c r="S62" s="114"/>
+      <c r="T62" s="114"/>
+      <c r="U62" s="114"/>
+      <c r="V62" s="114"/>
+      <c r="W62" s="114"/>
+      <c r="X62" s="114"/>
+      <c r="Y62" s="114"/>
+      <c r="Z62" s="114"/>
+      <c r="AA62" s="114"/>
+      <c r="AB62" s="114"/>
+      <c r="AC62" s="114"/>
+      <c r="AD62" s="114"/>
     </row>
     <row r="63" spans="2:43" ht="15" customHeight="1">
-      <c r="B63" s="116" t="s">
+      <c r="B63" s="115" t="s">
         <v>213</v>
       </c>
-      <c r="C63" s="116"/>
-      <c r="D63" s="116"/>
-      <c r="E63" s="116"/>
-      <c r="F63" s="116"/>
-      <c r="G63" s="116"/>
-      <c r="H63" s="116"/>
-      <c r="I63" s="116"/>
-      <c r="J63" s="116"/>
-      <c r="K63" s="116"/>
-      <c r="L63" s="116"/>
-      <c r="M63" s="116"/>
-      <c r="N63" s="116"/>
-      <c r="O63" s="116"/>
-      <c r="Q63" s="119"/>
-      <c r="R63" s="119"/>
-      <c r="S63" s="119"/>
-      <c r="T63" s="119"/>
-      <c r="U63" s="119"/>
-      <c r="V63" s="119"/>
-      <c r="W63" s="119"/>
-      <c r="X63" s="119"/>
-      <c r="Y63" s="119"/>
-      <c r="Z63" s="119"/>
-      <c r="AA63" s="119"/>
-      <c r="AB63" s="119"/>
-      <c r="AC63" s="119"/>
-      <c r="AD63" s="119"/>
+      <c r="C63" s="115"/>
+      <c r="D63" s="115"/>
+      <c r="E63" s="115"/>
+      <c r="F63" s="115"/>
+      <c r="G63" s="115"/>
+      <c r="H63" s="115"/>
+      <c r="I63" s="115"/>
+      <c r="J63" s="115"/>
+      <c r="K63" s="115"/>
+      <c r="L63" s="115"/>
+      <c r="M63" s="115"/>
+      <c r="N63" s="115"/>
+      <c r="O63" s="115"/>
+      <c r="Q63" s="114"/>
+      <c r="R63" s="114"/>
+      <c r="S63" s="114"/>
+      <c r="T63" s="114"/>
+      <c r="U63" s="114"/>
+      <c r="V63" s="114"/>
+      <c r="W63" s="114"/>
+      <c r="X63" s="114"/>
+      <c r="Y63" s="114"/>
+      <c r="Z63" s="114"/>
+      <c r="AA63" s="114"/>
+      <c r="AB63" s="114"/>
+      <c r="AC63" s="114"/>
+      <c r="AD63" s="114"/>
     </row>
     <row r="64" spans="2:43">
-      <c r="B64" s="116"/>
-      <c r="C64" s="116"/>
-      <c r="D64" s="116"/>
-      <c r="E64" s="116"/>
-      <c r="F64" s="116"/>
-      <c r="G64" s="116"/>
-      <c r="H64" s="116"/>
-      <c r="I64" s="116"/>
-      <c r="J64" s="116"/>
-      <c r="K64" s="116"/>
-      <c r="L64" s="116"/>
-      <c r="M64" s="116"/>
-      <c r="N64" s="116"/>
-      <c r="O64" s="116"/>
+      <c r="B64" s="115"/>
+      <c r="C64" s="115"/>
+      <c r="D64" s="115"/>
+      <c r="E64" s="115"/>
+      <c r="F64" s="115"/>
+      <c r="G64" s="115"/>
+      <c r="H64" s="115"/>
+      <c r="I64" s="115"/>
+      <c r="J64" s="115"/>
+      <c r="K64" s="115"/>
+      <c r="L64" s="115"/>
+      <c r="M64" s="115"/>
+      <c r="N64" s="115"/>
+      <c r="O64" s="115"/>
     </row>
     <row r="65" spans="2:30" ht="17.25">
-      <c r="B65" s="116"/>
-      <c r="C65" s="116"/>
-      <c r="D65" s="116"/>
-      <c r="E65" s="116"/>
-      <c r="F65" s="116"/>
-      <c r="G65" s="116"/>
-      <c r="H65" s="116"/>
-      <c r="I65" s="116"/>
-      <c r="J65" s="116"/>
-      <c r="K65" s="116"/>
-      <c r="L65" s="116"/>
-      <c r="M65" s="116"/>
-      <c r="N65" s="116"/>
-      <c r="O65" s="116"/>
+      <c r="B65" s="115"/>
+      <c r="C65" s="115"/>
+      <c r="D65" s="115"/>
+      <c r="E65" s="115"/>
+      <c r="F65" s="115"/>
+      <c r="G65" s="115"/>
+      <c r="H65" s="115"/>
+      <c r="I65" s="115"/>
+      <c r="J65" s="115"/>
+      <c r="K65" s="115"/>
+      <c r="L65" s="115"/>
+      <c r="M65" s="115"/>
+      <c r="N65" s="115"/>
+      <c r="O65" s="115"/>
       <c r="Q65" s="20" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="66" spans="2:30">
-      <c r="B66" s="116"/>
-      <c r="C66" s="116"/>
-      <c r="D66" s="116"/>
-      <c r="E66" s="116"/>
-      <c r="F66" s="116"/>
-      <c r="G66" s="116"/>
-      <c r="H66" s="116"/>
-      <c r="I66" s="116"/>
-      <c r="J66" s="116"/>
-      <c r="K66" s="116"/>
-      <c r="L66" s="116"/>
-      <c r="M66" s="116"/>
-      <c r="N66" s="116"/>
-      <c r="O66" s="116"/>
+      <c r="B66" s="115"/>
+      <c r="C66" s="115"/>
+      <c r="D66" s="115"/>
+      <c r="E66" s="115"/>
+      <c r="F66" s="115"/>
+      <c r="G66" s="115"/>
+      <c r="H66" s="115"/>
+      <c r="I66" s="115"/>
+      <c r="J66" s="115"/>
+      <c r="K66" s="115"/>
+      <c r="L66" s="115"/>
+      <c r="M66" s="115"/>
+      <c r="N66" s="115"/>
+      <c r="O66" s="115"/>
     </row>
     <row r="67" spans="2:30" ht="15" customHeight="1">
-      <c r="B67" s="119" t="s">
+      <c r="B67" s="114" t="s">
         <v>200</v>
       </c>
-      <c r="C67" s="119"/>
-      <c r="D67" s="119"/>
-      <c r="E67" s="119"/>
-      <c r="F67" s="119"/>
-      <c r="G67" s="119"/>
-      <c r="H67" s="119"/>
-      <c r="I67" s="119"/>
-      <c r="J67" s="119"/>
-      <c r="K67" s="119"/>
-      <c r="L67" s="119"/>
-      <c r="M67" s="119"/>
-      <c r="N67" s="119"/>
-      <c r="O67" s="119"/>
-      <c r="Q67" s="119" t="s">
+      <c r="C67" s="114"/>
+      <c r="D67" s="114"/>
+      <c r="E67" s="114"/>
+      <c r="F67" s="114"/>
+      <c r="G67" s="114"/>
+      <c r="H67" s="114"/>
+      <c r="I67" s="114"/>
+      <c r="J67" s="114"/>
+      <c r="K67" s="114"/>
+      <c r="L67" s="114"/>
+      <c r="M67" s="114"/>
+      <c r="N67" s="114"/>
+      <c r="O67" s="114"/>
+      <c r="Q67" s="114" t="s">
         <v>209</v>
       </c>
-      <c r="R67" s="119"/>
-      <c r="S67" s="119"/>
-      <c r="T67" s="119"/>
-      <c r="U67" s="119"/>
-      <c r="V67" s="119"/>
-      <c r="W67" s="119"/>
-      <c r="X67" s="119"/>
-      <c r="Y67" s="119"/>
-      <c r="Z67" s="119"/>
-      <c r="AA67" s="119"/>
-      <c r="AB67" s="119"/>
-      <c r="AC67" s="119"/>
-      <c r="AD67" s="119"/>
+      <c r="R67" s="114"/>
+      <c r="S67" s="114"/>
+      <c r="T67" s="114"/>
+      <c r="U67" s="114"/>
+      <c r="V67" s="114"/>
+      <c r="W67" s="114"/>
+      <c r="X67" s="114"/>
+      <c r="Y67" s="114"/>
+      <c r="Z67" s="114"/>
+      <c r="AA67" s="114"/>
+      <c r="AB67" s="114"/>
+      <c r="AC67" s="114"/>
+      <c r="AD67" s="114"/>
     </row>
     <row r="68" spans="2:30">
-      <c r="B68" s="119"/>
-      <c r="C68" s="119"/>
-      <c r="D68" s="119"/>
-      <c r="E68" s="119"/>
-      <c r="F68" s="119"/>
-      <c r="G68" s="119"/>
-      <c r="H68" s="119"/>
-      <c r="I68" s="119"/>
-      <c r="J68" s="119"/>
-      <c r="K68" s="119"/>
-      <c r="L68" s="119"/>
-      <c r="M68" s="119"/>
-      <c r="N68" s="119"/>
-      <c r="O68" s="119"/>
-      <c r="Q68" s="119"/>
-      <c r="R68" s="119"/>
-      <c r="S68" s="119"/>
-      <c r="T68" s="119"/>
-      <c r="U68" s="119"/>
-      <c r="V68" s="119"/>
-      <c r="W68" s="119"/>
-      <c r="X68" s="119"/>
-      <c r="Y68" s="119"/>
-      <c r="Z68" s="119"/>
-      <c r="AA68" s="119"/>
-      <c r="AB68" s="119"/>
-      <c r="AC68" s="119"/>
-      <c r="AD68" s="119"/>
+      <c r="B68" s="114"/>
+      <c r="C68" s="114"/>
+      <c r="D68" s="114"/>
+      <c r="E68" s="114"/>
+      <c r="F68" s="114"/>
+      <c r="G68" s="114"/>
+      <c r="H68" s="114"/>
+      <c r="I68" s="114"/>
+      <c r="J68" s="114"/>
+      <c r="K68" s="114"/>
+      <c r="L68" s="114"/>
+      <c r="M68" s="114"/>
+      <c r="N68" s="114"/>
+      <c r="O68" s="114"/>
+      <c r="Q68" s="114"/>
+      <c r="R68" s="114"/>
+      <c r="S68" s="114"/>
+      <c r="T68" s="114"/>
+      <c r="U68" s="114"/>
+      <c r="V68" s="114"/>
+      <c r="W68" s="114"/>
+      <c r="X68" s="114"/>
+      <c r="Y68" s="114"/>
+      <c r="Z68" s="114"/>
+      <c r="AA68" s="114"/>
+      <c r="AB68" s="114"/>
+      <c r="AC68" s="114"/>
+      <c r="AD68" s="114"/>
     </row>
     <row r="69" spans="2:30">
-      <c r="Q69" s="119"/>
-      <c r="R69" s="119"/>
-      <c r="S69" s="119"/>
-      <c r="T69" s="119"/>
-      <c r="U69" s="119"/>
-      <c r="V69" s="119"/>
-      <c r="W69" s="119"/>
-      <c r="X69" s="119"/>
-      <c r="Y69" s="119"/>
-      <c r="Z69" s="119"/>
-      <c r="AA69" s="119"/>
-      <c r="AB69" s="119"/>
-      <c r="AC69" s="119"/>
-      <c r="AD69" s="119"/>
+      <c r="Q69" s="114"/>
+      <c r="R69" s="114"/>
+      <c r="S69" s="114"/>
+      <c r="T69" s="114"/>
+      <c r="U69" s="114"/>
+      <c r="V69" s="114"/>
+      <c r="W69" s="114"/>
+      <c r="X69" s="114"/>
+      <c r="Y69" s="114"/>
+      <c r="Z69" s="114"/>
+      <c r="AA69" s="114"/>
+      <c r="AB69" s="114"/>
+      <c r="AC69" s="114"/>
+      <c r="AD69" s="114"/>
     </row>
     <row r="70" spans="2:30" ht="17.25">
       <c r="B70" s="10" t="s">
@@ -4202,196 +4202,207 @@
       </c>
     </row>
     <row r="73" spans="2:30">
-      <c r="Q73" s="116" t="s">
+      <c r="Q73" s="115" t="s">
         <v>203</v>
       </c>
-      <c r="R73" s="116"/>
-      <c r="S73" s="116"/>
-      <c r="T73" s="116"/>
-      <c r="U73" s="116"/>
-      <c r="V73" s="116"/>
-      <c r="W73" s="116"/>
-      <c r="X73" s="116"/>
-      <c r="Y73" s="116"/>
-      <c r="Z73" s="116"/>
-      <c r="AA73" s="116"/>
-      <c r="AB73" s="116"/>
-      <c r="AC73" s="116"/>
-      <c r="AD73" s="116"/>
+      <c r="R73" s="115"/>
+      <c r="S73" s="115"/>
+      <c r="T73" s="115"/>
+      <c r="U73" s="115"/>
+      <c r="V73" s="115"/>
+      <c r="W73" s="115"/>
+      <c r="X73" s="115"/>
+      <c r="Y73" s="115"/>
+      <c r="Z73" s="115"/>
+      <c r="AA73" s="115"/>
+      <c r="AB73" s="115"/>
+      <c r="AC73" s="115"/>
+      <c r="AD73" s="115"/>
     </row>
     <row r="74" spans="2:30">
-      <c r="Q74" s="116"/>
-      <c r="R74" s="116"/>
-      <c r="S74" s="116"/>
-      <c r="T74" s="116"/>
-      <c r="U74" s="116"/>
-      <c r="V74" s="116"/>
-      <c r="W74" s="116"/>
-      <c r="X74" s="116"/>
-      <c r="Y74" s="116"/>
-      <c r="Z74" s="116"/>
-      <c r="AA74" s="116"/>
-      <c r="AB74" s="116"/>
-      <c r="AC74" s="116"/>
-      <c r="AD74" s="116"/>
+      <c r="Q74" s="115"/>
+      <c r="R74" s="115"/>
+      <c r="S74" s="115"/>
+      <c r="T74" s="115"/>
+      <c r="U74" s="115"/>
+      <c r="V74" s="115"/>
+      <c r="W74" s="115"/>
+      <c r="X74" s="115"/>
+      <c r="Y74" s="115"/>
+      <c r="Z74" s="115"/>
+      <c r="AA74" s="115"/>
+      <c r="AB74" s="115"/>
+      <c r="AC74" s="115"/>
+      <c r="AD74" s="115"/>
     </row>
     <row r="75" spans="2:30" ht="15" customHeight="1">
-      <c r="Q75" s="116"/>
-      <c r="R75" s="116"/>
-      <c r="S75" s="116"/>
-      <c r="T75" s="116"/>
-      <c r="U75" s="116"/>
-      <c r="V75" s="116"/>
-      <c r="W75" s="116"/>
-      <c r="X75" s="116"/>
-      <c r="Y75" s="116"/>
-      <c r="Z75" s="116"/>
-      <c r="AA75" s="116"/>
-      <c r="AB75" s="116"/>
-      <c r="AC75" s="116"/>
-      <c r="AD75" s="116"/>
+      <c r="Q75" s="115"/>
+      <c r="R75" s="115"/>
+      <c r="S75" s="115"/>
+      <c r="T75" s="115"/>
+      <c r="U75" s="115"/>
+      <c r="V75" s="115"/>
+      <c r="W75" s="115"/>
+      <c r="X75" s="115"/>
+      <c r="Y75" s="115"/>
+      <c r="Z75" s="115"/>
+      <c r="AA75" s="115"/>
+      <c r="AB75" s="115"/>
+      <c r="AC75" s="115"/>
+      <c r="AD75" s="115"/>
     </row>
     <row r="76" spans="2:30">
-      <c r="Q76" s="116"/>
-      <c r="R76" s="116"/>
-      <c r="S76" s="116"/>
-      <c r="T76" s="116"/>
-      <c r="U76" s="116"/>
-      <c r="V76" s="116"/>
-      <c r="W76" s="116"/>
-      <c r="X76" s="116"/>
-      <c r="Y76" s="116"/>
-      <c r="Z76" s="116"/>
-      <c r="AA76" s="116"/>
-      <c r="AB76" s="116"/>
-      <c r="AC76" s="116"/>
-      <c r="AD76" s="116"/>
+      <c r="Q76" s="115"/>
+      <c r="R76" s="115"/>
+      <c r="S76" s="115"/>
+      <c r="T76" s="115"/>
+      <c r="U76" s="115"/>
+      <c r="V76" s="115"/>
+      <c r="W76" s="115"/>
+      <c r="X76" s="115"/>
+      <c r="Y76" s="115"/>
+      <c r="Z76" s="115"/>
+      <c r="AA76" s="115"/>
+      <c r="AB76" s="115"/>
+      <c r="AC76" s="115"/>
+      <c r="AD76" s="115"/>
     </row>
     <row r="77" spans="2:30">
-      <c r="Q77" s="116"/>
-      <c r="R77" s="116"/>
-      <c r="S77" s="116"/>
-      <c r="T77" s="116"/>
-      <c r="U77" s="116"/>
-      <c r="V77" s="116"/>
-      <c r="W77" s="116"/>
-      <c r="X77" s="116"/>
-      <c r="Y77" s="116"/>
-      <c r="Z77" s="116"/>
-      <c r="AA77" s="116"/>
-      <c r="AB77" s="116"/>
-      <c r="AC77" s="116"/>
-      <c r="AD77" s="116"/>
+      <c r="Q77" s="115"/>
+      <c r="R77" s="115"/>
+      <c r="S77" s="115"/>
+      <c r="T77" s="115"/>
+      <c r="U77" s="115"/>
+      <c r="V77" s="115"/>
+      <c r="W77" s="115"/>
+      <c r="X77" s="115"/>
+      <c r="Y77" s="115"/>
+      <c r="Z77" s="115"/>
+      <c r="AA77" s="115"/>
+      <c r="AB77" s="115"/>
+      <c r="AC77" s="115"/>
+      <c r="AD77" s="115"/>
     </row>
     <row r="79" spans="2:30" ht="17.25">
-      <c r="B79" s="114" t="s">
+      <c r="B79" s="122" t="s">
         <v>101</v>
       </c>
-      <c r="C79" s="114"/>
-      <c r="D79" s="114"/>
-      <c r="E79" s="114"/>
-      <c r="F79" s="114"/>
-      <c r="G79" s="114"/>
-      <c r="H79" s="114"/>
-      <c r="I79" s="114"/>
-      <c r="J79" s="114"/>
-      <c r="K79" s="114"/>
-      <c r="L79" s="114"/>
-      <c r="M79" s="114"/>
-      <c r="N79" s="114"/>
-      <c r="O79" s="114"/>
+      <c r="C79" s="122"/>
+      <c r="D79" s="122"/>
+      <c r="E79" s="122"/>
+      <c r="F79" s="122"/>
+      <c r="G79" s="122"/>
+      <c r="H79" s="122"/>
+      <c r="I79" s="122"/>
+      <c r="J79" s="122"/>
+      <c r="K79" s="122"/>
+      <c r="L79" s="122"/>
+      <c r="M79" s="122"/>
+      <c r="N79" s="122"/>
+      <c r="O79" s="122"/>
       <c r="Q79" s="20" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="81" spans="2:30" ht="15" customHeight="1">
-      <c r="B81" s="119" t="s">
+      <c r="B81" s="114" t="s">
         <v>193</v>
       </c>
-      <c r="C81" s="119"/>
-      <c r="D81" s="119"/>
-      <c r="E81" s="119"/>
-      <c r="F81" s="119"/>
-      <c r="G81" s="119"/>
-      <c r="H81" s="119"/>
-      <c r="I81" s="119"/>
-      <c r="J81" s="119"/>
-      <c r="K81" s="119"/>
-      <c r="L81" s="119"/>
-      <c r="M81" s="119"/>
-      <c r="N81" s="119"/>
-      <c r="O81" s="119"/>
-      <c r="Q81" s="116" t="s">
+      <c r="C81" s="114"/>
+      <c r="D81" s="114"/>
+      <c r="E81" s="114"/>
+      <c r="F81" s="114"/>
+      <c r="G81" s="114"/>
+      <c r="H81" s="114"/>
+      <c r="I81" s="114"/>
+      <c r="J81" s="114"/>
+      <c r="K81" s="114"/>
+      <c r="L81" s="114"/>
+      <c r="M81" s="114"/>
+      <c r="N81" s="114"/>
+      <c r="O81" s="114"/>
+      <c r="Q81" s="115" t="s">
         <v>202</v>
       </c>
-      <c r="R81" s="116"/>
-      <c r="S81" s="116"/>
-      <c r="T81" s="116"/>
-      <c r="U81" s="116"/>
-      <c r="V81" s="116"/>
-      <c r="W81" s="116"/>
-      <c r="X81" s="116"/>
-      <c r="Y81" s="116"/>
-      <c r="Z81" s="116"/>
-      <c r="AA81" s="116"/>
-      <c r="AB81" s="116"/>
-      <c r="AC81" s="116"/>
-      <c r="AD81" s="116"/>
+      <c r="R81" s="115"/>
+      <c r="S81" s="115"/>
+      <c r="T81" s="115"/>
+      <c r="U81" s="115"/>
+      <c r="V81" s="115"/>
+      <c r="W81" s="115"/>
+      <c r="X81" s="115"/>
+      <c r="Y81" s="115"/>
+      <c r="Z81" s="115"/>
+      <c r="AA81" s="115"/>
+      <c r="AB81" s="115"/>
+      <c r="AC81" s="115"/>
+      <c r="AD81" s="115"/>
     </row>
     <row r="82" spans="2:30">
-      <c r="B82" s="119"/>
-      <c r="C82" s="119"/>
-      <c r="D82" s="119"/>
-      <c r="E82" s="119"/>
-      <c r="F82" s="119"/>
-      <c r="G82" s="119"/>
-      <c r="H82" s="119"/>
-      <c r="I82" s="119"/>
-      <c r="J82" s="119"/>
-      <c r="K82" s="119"/>
-      <c r="L82" s="119"/>
-      <c r="M82" s="119"/>
-      <c r="N82" s="119"/>
-      <c r="O82" s="119"/>
-      <c r="Q82" s="116"/>
-      <c r="R82" s="116"/>
-      <c r="S82" s="116"/>
-      <c r="T82" s="116"/>
-      <c r="U82" s="116"/>
-      <c r="V82" s="116"/>
-      <c r="W82" s="116"/>
-      <c r="X82" s="116"/>
-      <c r="Y82" s="116"/>
-      <c r="Z82" s="116"/>
-      <c r="AA82" s="116"/>
-      <c r="AB82" s="116"/>
-      <c r="AC82" s="116"/>
-      <c r="AD82" s="116"/>
+      <c r="B82" s="114"/>
+      <c r="C82" s="114"/>
+      <c r="D82" s="114"/>
+      <c r="E82" s="114"/>
+      <c r="F82" s="114"/>
+      <c r="G82" s="114"/>
+      <c r="H82" s="114"/>
+      <c r="I82" s="114"/>
+      <c r="J82" s="114"/>
+      <c r="K82" s="114"/>
+      <c r="L82" s="114"/>
+      <c r="M82" s="114"/>
+      <c r="N82" s="114"/>
+      <c r="O82" s="114"/>
+      <c r="Q82" s="115"/>
+      <c r="R82" s="115"/>
+      <c r="S82" s="115"/>
+      <c r="T82" s="115"/>
+      <c r="U82" s="115"/>
+      <c r="V82" s="115"/>
+      <c r="W82" s="115"/>
+      <c r="X82" s="115"/>
+      <c r="Y82" s="115"/>
+      <c r="Z82" s="115"/>
+      <c r="AA82" s="115"/>
+      <c r="AB82" s="115"/>
+      <c r="AC82" s="115"/>
+      <c r="AD82" s="115"/>
     </row>
     <row r="83" spans="2:30">
-      <c r="Q83" s="116"/>
-      <c r="R83" s="116"/>
-      <c r="S83" s="116"/>
-      <c r="T83" s="116"/>
-      <c r="U83" s="116"/>
-      <c r="V83" s="116"/>
-      <c r="W83" s="116"/>
-      <c r="X83" s="116"/>
-      <c r="Y83" s="116"/>
-      <c r="Z83" s="116"/>
-      <c r="AA83" s="116"/>
-      <c r="AB83" s="116"/>
-      <c r="AC83" s="116"/>
-      <c r="AD83" s="116"/>
+      <c r="Q83" s="115"/>
+      <c r="R83" s="115"/>
+      <c r="S83" s="115"/>
+      <c r="T83" s="115"/>
+      <c r="U83" s="115"/>
+      <c r="V83" s="115"/>
+      <c r="W83" s="115"/>
+      <c r="X83" s="115"/>
+      <c r="Y83" s="115"/>
+      <c r="Z83" s="115"/>
+      <c r="AA83" s="115"/>
+      <c r="AB83" s="115"/>
+      <c r="AC83" s="115"/>
+      <c r="AD83" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B81:O82"/>
-    <mergeCell ref="Q62:AD63"/>
-    <mergeCell ref="B63:O66"/>
-    <mergeCell ref="B67:O68"/>
-    <mergeCell ref="Q73:AD77"/>
-    <mergeCell ref="Q81:AD83"/>
+    <mergeCell ref="B58:O58"/>
+    <mergeCell ref="B79:O79"/>
+    <mergeCell ref="Q58:AD58"/>
+    <mergeCell ref="B60:O61"/>
+    <mergeCell ref="V48:Z48"/>
+    <mergeCell ref="S50:AB50"/>
+    <mergeCell ref="Q67:AD69"/>
+    <mergeCell ref="B50:O51"/>
+    <mergeCell ref="S33:AB34"/>
+    <mergeCell ref="S37:AB38"/>
+    <mergeCell ref="S42:AB42"/>
+    <mergeCell ref="S45:AB46"/>
+    <mergeCell ref="B55:O56"/>
+    <mergeCell ref="B33:N34"/>
+    <mergeCell ref="B38:O39"/>
+    <mergeCell ref="B41:O41"/>
+    <mergeCell ref="B45:O46"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B4:O5"/>
     <mergeCell ref="B8:O9"/>
@@ -4408,23 +4419,12 @@
     <mergeCell ref="V40:Z40"/>
     <mergeCell ref="S29:AB29"/>
     <mergeCell ref="S26:AB26"/>
-    <mergeCell ref="S33:AB34"/>
-    <mergeCell ref="S37:AB38"/>
-    <mergeCell ref="S42:AB42"/>
-    <mergeCell ref="S45:AB46"/>
-    <mergeCell ref="B55:O56"/>
-    <mergeCell ref="B33:N34"/>
-    <mergeCell ref="B38:O39"/>
-    <mergeCell ref="B41:O41"/>
-    <mergeCell ref="B45:O46"/>
-    <mergeCell ref="B58:O58"/>
-    <mergeCell ref="B79:O79"/>
-    <mergeCell ref="Q58:AD58"/>
-    <mergeCell ref="B60:O61"/>
-    <mergeCell ref="V48:Z48"/>
-    <mergeCell ref="S50:AB50"/>
-    <mergeCell ref="Q67:AD69"/>
-    <mergeCell ref="B50:O51"/>
+    <mergeCell ref="B81:O82"/>
+    <mergeCell ref="Q62:AD63"/>
+    <mergeCell ref="B63:O66"/>
+    <mergeCell ref="B67:O68"/>
+    <mergeCell ref="Q73:AD77"/>
+    <mergeCell ref="Q81:AD83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6008,10 +6008,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6028,7 +6028,7 @@
     <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="31" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:12" s="31" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="33" t="s">
         <v>148</v>
       </c>
@@ -6056,7 +6056,7 @@
       <c r="I1" s="32"/>
       <c r="J1" s="32"/>
     </row>
-    <row r="2" spans="1:10" s="31" customFormat="1" ht="15.75" thickTop="1">
+    <row r="2" spans="1:12" s="31" customFormat="1" ht="15.75" thickTop="1">
       <c r="A2" s="35">
         <v>1</v>
       </c>
@@ -6081,10 +6081,26 @@
         <v>95</v>
       </c>
       <c r="H2" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="31" customFormat="1">
+        <v>1.5226168411632972</v>
+      </c>
+      <c r="I2" s="31">
+        <f>+C2/AVERAGE($C$2:$C$26)</f>
+        <v>3.5573169354033003</v>
+      </c>
+      <c r="J2" s="31">
+        <f>MAX(I2:I26)-MIN(I2:I26)</f>
+        <v>19.175459952522917</v>
+      </c>
+      <c r="K2" s="31">
+        <f>J3/J2</f>
+        <v>6.2579985198327193E-2</v>
+      </c>
+      <c r="L2" s="31">
+        <f>+$K$2*I2+(2.5-$J$3)</f>
+        <v>1.5226168411632972</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="31" customFormat="1">
       <c r="A3" s="35">
         <v>2</v>
       </c>
@@ -6109,10 +6125,22 @@
         <v>94</v>
       </c>
       <c r="H3" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="31" customFormat="1">
+        <v>1.6355347290970543</v>
+      </c>
+      <c r="I3" s="31">
+        <f t="shared" ref="I3:I26" si="1">+E3/AVERAGE($E$2:$E$26)</f>
+        <v>5.3616939670676587</v>
+      </c>
+      <c r="J3" s="31">
+        <f>2.5-1.3</f>
+        <v>1.2</v>
+      </c>
+      <c r="L3" s="31">
+        <f t="shared" ref="L3:L26" si="2">+$K$2*I3+(2.5-$J$3)</f>
+        <v>1.6355347290970543</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="31" customFormat="1">
       <c r="A4" s="35">
         <v>3</v>
       </c>
@@ -6136,10 +6164,18 @@
         <v>42</v>
       </c>
       <c r="H4" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="31" customFormat="1">
+        <v>1.3016445296493757</v>
+      </c>
+      <c r="I4" s="31">
+        <f t="shared" si="1"/>
+        <v>2.62788436936169E-2</v>
+      </c>
+      <c r="L4" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3016445296493757</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="31" customFormat="1">
       <c r="A5" s="35">
         <v>4</v>
       </c>
@@ -6163,10 +6199,18 @@
         <v>43</v>
       </c>
       <c r="H5" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="31" customFormat="1">
+        <v>1.3020145571735886</v>
+      </c>
+      <c r="I5" s="31">
+        <f t="shared" si="1"/>
+        <v>3.2191717003511783E-2</v>
+      </c>
+      <c r="L5" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3020145571735886</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="31" customFormat="1">
       <c r="A6" s="35">
         <v>5</v>
       </c>
@@ -6190,10 +6234,18 @@
         <v>93</v>
       </c>
       <c r="H6" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="31" customFormat="1">
+        <v>2.5000942000884692</v>
+      </c>
+      <c r="I6" s="31">
+        <f t="shared" si="1"/>
+        <v>19.176965227542883</v>
+      </c>
+      <c r="L6" s="31">
+        <f t="shared" si="2"/>
+        <v>2.5000942000884692</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="31" customFormat="1">
       <c r="A7" s="35">
         <v>6</v>
       </c>
@@ -6217,10 +6269,18 @@
         <v>41</v>
       </c>
       <c r="H7" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="31" customFormat="1">
+        <v>1.3009800456274476</v>
+      </c>
+      <c r="I7" s="31">
+        <f t="shared" si="1"/>
+        <v>1.5660688067304182E-2</v>
+      </c>
+      <c r="L7" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3009800456274476</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="31" customFormat="1">
       <c r="A8" s="35">
         <v>7</v>
       </c>
@@ -6244,10 +6304,18 @@
         <v>44</v>
       </c>
       <c r="H8" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="31" customFormat="1">
+        <v>1.3053929401236657</v>
+      </c>
+      <c r="I8" s="31">
+        <f t="shared" si="1"/>
+        <v>8.6176756139753355E-2</v>
+      </c>
+      <c r="L8" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3053929401236657</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="31" customFormat="1">
       <c r="A9" s="35">
         <v>8</v>
       </c>
@@ -6271,10 +6339,18 @@
         <v>43</v>
       </c>
       <c r="H9" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="31" customFormat="1">
+        <v>1.3013159550225286</v>
+      </c>
+      <c r="I9" s="31">
+        <f t="shared" si="1"/>
+        <v>2.1028369028180349E-2</v>
+      </c>
+      <c r="L9" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3013159550225286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="31" customFormat="1">
       <c r="A10" s="35">
         <v>9</v>
       </c>
@@ -6298,10 +6374,18 @@
         <v>44</v>
       </c>
       <c r="H10" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="31" customFormat="1">
+        <v>1.3006553970942678</v>
+      </c>
+      <c r="I10" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0472950611776718E-2</v>
+      </c>
+      <c r="L10" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3006553970942678</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="31" customFormat="1">
       <c r="A11" s="35">
         <v>10</v>
       </c>
@@ -6325,10 +6409,18 @@
         <v>43</v>
       </c>
       <c r="H11" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="31" customFormat="1">
+        <v>1.303100534032853</v>
+      </c>
+      <c r="I11" s="31">
+        <f t="shared" si="1"/>
+        <v>4.9545138482003079E-2</v>
+      </c>
+      <c r="L11" s="31">
+        <f t="shared" si="2"/>
+        <v>1.303100534032853</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="31" customFormat="1">
       <c r="A12" s="35">
         <v>11</v>
       </c>
@@ -6352,10 +6444,18 @@
         <v>43</v>
       </c>
       <c r="H12" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="31" customFormat="1">
+        <v>1.3008883866631449</v>
+      </c>
+      <c r="I12" s="31">
+        <f>+E12/AVERAGE($E$2:$E$26)</f>
+        <v>1.41960190679076E-2</v>
+      </c>
+      <c r="L12" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3008883866631449</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="31" customFormat="1">
       <c r="A13" s="35">
         <v>12</v>
       </c>
@@ -6379,10 +6479,18 @@
         <v>43</v>
       </c>
       <c r="H13" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="31" customFormat="1">
+        <v>1.3009439621802783</v>
+      </c>
+      <c r="I13" s="31">
+        <f t="shared" si="1"/>
+        <v>1.5084090820518228E-2</v>
+      </c>
+      <c r="L13" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3009439621802783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="31" customFormat="1">
       <c r="A14" s="35">
         <v>13</v>
       </c>
@@ -6406,10 +6514,18 @@
         <v>44</v>
       </c>
       <c r="H14" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="31" customFormat="1">
+        <v>1.3005376532300745</v>
+      </c>
+      <c r="I14" s="31">
+        <f t="shared" si="1"/>
+        <v>8.5914566513635611E-3</v>
+      </c>
+      <c r="L14" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3005376532300745</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="31" customFormat="1">
       <c r="A15" s="35">
         <v>14</v>
       </c>
@@ -6433,10 +6549,18 @@
         <v>41</v>
       </c>
       <c r="H15" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="31" customFormat="1">
+        <v>1.3006371962629926</v>
+      </c>
+      <c r="I15" s="31">
+        <f t="shared" si="1"/>
+        <v>1.0182109519091148E-2</v>
+      </c>
+      <c r="L15" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3006371962629926</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="31" customFormat="1">
       <c r="A16" s="35">
         <v>15</v>
       </c>
@@ -6460,10 +6584,18 @@
         <v>44</v>
       </c>
       <c r="H16" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="31" customFormat="1">
+        <v>1.3010611886405909</v>
+      </c>
+      <c r="I16" s="31">
+        <f t="shared" si="1"/>
+        <v>1.6957316899768048E-2</v>
+      </c>
+      <c r="L16" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3010611886405909</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="31" customFormat="1">
       <c r="A17" s="35">
         <v>16</v>
       </c>
@@ -6487,10 +6619,18 @@
         <v>45</v>
       </c>
       <c r="H17" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="31" customFormat="1">
+        <v>1.300263865031827</v>
+      </c>
+      <c r="I17" s="31">
+        <f t="shared" si="1"/>
+        <v>4.2164444588902008E-3</v>
+      </c>
+      <c r="L17" s="31">
+        <f t="shared" si="2"/>
+        <v>1.300263865031827</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="31" customFormat="1">
       <c r="A18" s="35">
         <v>17</v>
       </c>
@@ -6514,10 +6654,18 @@
         <v>45</v>
       </c>
       <c r="H18" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="31" customFormat="1">
+        <v>1.3004914952263631</v>
+      </c>
+      <c r="I18" s="31">
+        <f t="shared" si="1"/>
+        <v>7.853872524985173E-3</v>
+      </c>
+      <c r="L18" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3004914952263631</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="31" customFormat="1">
       <c r="A19" s="35">
         <v>18</v>
       </c>
@@ -6541,10 +6689,18 @@
         <v>43</v>
       </c>
       <c r="H19" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="31" customFormat="1">
+        <v>1.3006170556755365</v>
+      </c>
+      <c r="I19" s="31">
+        <f t="shared" si="1"/>
+        <v>9.8602719956064899E-3</v>
+      </c>
+      <c r="L19" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3006170556755365</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="31" customFormat="1">
       <c r="A20" s="35">
         <v>19</v>
       </c>
@@ -6568,10 +6724,18 @@
         <v>45</v>
       </c>
       <c r="H20" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="31" customFormat="1">
+        <v>1.3001900553421324</v>
+      </c>
+      <c r="I20" s="31">
+        <f t="shared" si="1"/>
+        <v>3.0369988348518751E-3</v>
+      </c>
+      <c r="L20" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3001900553421324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="31" customFormat="1">
       <c r="A21" s="35">
         <v>20</v>
       </c>
@@ -6595,10 +6759,18 @@
         <v>41</v>
       </c>
       <c r="H21" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="31" customFormat="1">
+        <v>1.3004724701627346</v>
+      </c>
+      <c r="I21" s="31">
+        <f t="shared" si="1"/>
+        <v>7.5498605702304534E-3</v>
+      </c>
+      <c r="L21" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3004724701627346</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="31" customFormat="1">
       <c r="A22" s="35">
         <v>21</v>
       </c>
@@ -6622,10 +6794,18 @@
         <v>44</v>
       </c>
       <c r="H22" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="31" customFormat="1">
+        <v>1.3003007011797021</v>
+      </c>
+      <c r="I22" s="31">
+        <f t="shared" si="1"/>
+        <v>4.8050695242102242E-3</v>
+      </c>
+      <c r="L22" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3003007011797021</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="31" customFormat="1">
       <c r="A23" s="35">
         <v>22</v>
       </c>
@@ -6649,10 +6829,18 @@
         <v>44</v>
       </c>
       <c r="H23" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="31" customFormat="1">
+        <v>1.3003122500852042</v>
+      </c>
+      <c r="I23" s="31">
+        <f t="shared" si="1"/>
+        <v>4.9896158366721961E-3</v>
+      </c>
+      <c r="L23" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3003122500852042</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="31" customFormat="1">
       <c r="A24" s="35">
         <v>23</v>
       </c>
@@ -6676,10 +6864,18 @@
         <v>45</v>
       </c>
       <c r="H24" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="31" customFormat="1">
+        <v>1.3001865090303404</v>
+      </c>
+      <c r="I24" s="31">
+        <f t="shared" si="1"/>
+        <v>2.9803303683967825E-3</v>
+      </c>
+      <c r="L24" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3001865090303404</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="31" customFormat="1">
       <c r="A25" s="35">
         <v>24</v>
       </c>
@@ -6703,10 +6899,18 @@
         <v>45</v>
       </c>
       <c r="H25" s="38">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="31" customFormat="1">
+        <v>1.300094200088469</v>
+      </c>
+      <c r="I25" s="31">
+        <f t="shared" si="1"/>
+        <v>1.5052750199671203E-3</v>
+      </c>
+      <c r="L25" s="31">
+        <f t="shared" si="2"/>
+        <v>1.300094200088469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="31" customFormat="1">
       <c r="A26" s="35">
         <v>25</v>
       </c>
@@ -6730,7 +6934,15 @@
         <v>45</v>
       </c>
       <c r="H26" s="38">
-        <v>2.5</v>
+        <v>1.3004946295702993</v>
+      </c>
+      <c r="I26" s="31">
+        <f t="shared" si="1"/>
+        <v>7.9039579305052385E-3</v>
+      </c>
+      <c r="L26" s="31">
+        <f t="shared" si="2"/>
+        <v>1.3004946295702993</v>
       </c>
     </row>
   </sheetData>
@@ -70026,7 +70238,7 @@
   </sheetPr>
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>